<commit_message>
add new feature proveedor facturas y productos
</commit_message>
<xml_diff>
--- a/MODULOS SISTEMA MR.xlsx
+++ b/MODULOS SISTEMA MR.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\api_mrimnova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78F85DC-DBB9-46C4-B170-D2A0EE81B87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC9976-59B3-4641-99EC-388A05317B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{ECD15C7F-3157-4274-92FE-24997BBCF2C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECD15C7F-3157-4274-92FE-24997BBCF2C6}"/>
   </bookViews>
   <sheets>
     <sheet name="MODULOS" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
-    <sheet name="BASE DE DATOS" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="BASE DE DATOS" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
   <si>
     <t>MÓDULOS MR</t>
   </si>
@@ -334,6 +336,42 @@
   </si>
   <si>
     <t>F103 (Importar de Bizlinkz) - video vig</t>
+  </si>
+  <si>
+    <t>1.- Definir campos proveedores</t>
+  </si>
+  <si>
+    <t>2.- Los productos pueden estar definidos a 1 o mas proveedores?</t>
+  </si>
+  <si>
+    <t>3.- Campos de los productos validar</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>plazo</t>
+  </si>
+  <si>
+    <t>cuota</t>
+  </si>
+  <si>
+    <t>Video Vigilancia 24/7</t>
+  </si>
+  <si>
+    <t>2 camaras</t>
+  </si>
+  <si>
+    <t>18 meses</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
@@ -542,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -588,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,7 +947,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,6 +1257,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB631C8-DF2E-4B68-B31E-B78B090575D6}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1335759B-946A-4163-9D55-40FA36D53B3A}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -1376,12 +1453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30A486F-41CF-4933-92FD-D81DF28DEC16}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,4 +1619,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40366489-87FD-4DEC-A585-B81EE188AF59}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update ventas - productos
</commit_message>
<xml_diff>
--- a/MODULOS SISTEMA MR.xlsx
+++ b/MODULOS SISTEMA MR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\api_mrimnova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC9976-59B3-4641-99EC-388A05317B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA41080-9898-48F6-9428-4D497C36C3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECD15C7F-3157-4274-92FE-24997BBCF2C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ECD15C7F-3157-4274-92FE-24997BBCF2C6}"/>
   </bookViews>
   <sheets>
     <sheet name="MODULOS" sheetId="1" r:id="rId1"/>
@@ -618,6 +618,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -626,9 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6235EE11-D643-446D-B21D-5B4353AF5B3D}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,13 +962,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,21 +1625,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40366489-87FD-4DEC-A585-B81EE188AF59}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       <c r="A2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       <c r="A3" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>100</v>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
       <c r="A5" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>